<commit_message>
changing velocity gradient calculation
</commit_message>
<xml_diff>
--- a/matlab/preform/IRprofile.xlsx
+++ b/matlab/preform/IRprofile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="IR profile" sheetId="1" state="visible" r:id="rId2"/>
@@ -202,7 +202,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -522,34 +522,34 @@
                   <c:v>97.45</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>97.45</c:v>
+                  <c:v>97.25</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>97.45</c:v>
+                  <c:v>97.05</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>97.45</c:v>
+                  <c:v>96.85</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>97.45</c:v>
+                  <c:v>96.65</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>97.35</c:v>
+                  <c:v>96.45</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>97.1</c:v>
+                  <c:v>96.25</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>96.85</c:v>
+                  <c:v>96.05</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>96.6</c:v>
+                  <c:v>95.85</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>96.35</c:v>
+                  <c:v>95.65</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>96.1</c:v>
+                  <c:v>95.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -867,45 +867,45 @@
                   <c:v>97.45</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>97.45</c:v>
+                  <c:v>97.25</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>97.45</c:v>
+                  <c:v>97.05</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>97.45</c:v>
+                  <c:v>96.85</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>97.45</c:v>
+                  <c:v>96.65</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>97.35</c:v>
+                  <c:v>96.45</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>97.1</c:v>
+                  <c:v>96.25</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>96.85</c:v>
+                  <c:v>96.05</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>96.6</c:v>
+                  <c:v>95.85</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>96.35</c:v>
+                  <c:v>95.65</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>96.1</c:v>
+                  <c:v>95.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="7807197"/>
-        <c:axId val="32089143"/>
+        <c:axId val="15287847"/>
+        <c:axId val="33887258"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="7807197"/>
+        <c:axId val="15287847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -942,12 +942,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32089143"/>
+        <c:crossAx val="33887258"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="32089143"/>
+        <c:axId val="33887258"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120"/>
@@ -995,7 +995,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7807197"/>
+        <c:crossAx val="15287847"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1032,7 +1032,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1703,67 +1703,67 @@
                   <c:v>97.45</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>97.45</c:v>
+                  <c:v>97.25</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>97.45</c:v>
+                  <c:v>97.05</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>97.45</c:v>
+                  <c:v>96.85</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>97.45</c:v>
+                  <c:v>96.65</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>97.35</c:v>
+                  <c:v>96.45</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>97.1</c:v>
+                  <c:v>96.25</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>96.85</c:v>
+                  <c:v>96.05</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>96.6</c:v>
+                  <c:v>95.85</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>96.35</c:v>
+                  <c:v>95.65</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>96.1</c:v>
+                  <c:v>95.45</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>95.85</c:v>
+                  <c:v>95.25</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>95.6</c:v>
+                  <c:v>95.05</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>95.35</c:v>
+                  <c:v>94.85</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>94.35</c:v>
+                  <c:v>93.85</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>93.35</c:v>
+                  <c:v>92.85</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>92.35</c:v>
+                  <c:v>91.85</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>91.35</c:v>
+                  <c:v>90.85</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>90.35</c:v>
+                  <c:v>89.85</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>89.35</c:v>
+                  <c:v>88.85</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>88.35</c:v>
+                  <c:v>87.85</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>87.35</c:v>
+                  <c:v>86.85</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v/>
@@ -2378,78 +2378,78 @@
                   <c:v>97.45</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>97.45</c:v>
+                  <c:v>97.25</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>97.45</c:v>
+                  <c:v>97.05</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>97.45</c:v>
+                  <c:v>96.85</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>97.45</c:v>
+                  <c:v>96.65</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>97.35</c:v>
+                  <c:v>96.45</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>97.1</c:v>
+                  <c:v>96.25</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>96.85</c:v>
+                  <c:v>96.05</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>96.6</c:v>
+                  <c:v>95.85</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>96.35</c:v>
+                  <c:v>95.65</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>96.1</c:v>
+                  <c:v>95.45</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>95.85</c:v>
+                  <c:v>95.25</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>95.6</c:v>
+                  <c:v>95.05</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>95.35</c:v>
+                  <c:v>94.85</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>94.35</c:v>
+                  <c:v>93.85</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>93.35</c:v>
+                  <c:v>92.85</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>92.35</c:v>
+                  <c:v>91.85</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>91.35</c:v>
+                  <c:v>90.85</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>90.35</c:v>
+                  <c:v>89.85</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>89.35</c:v>
+                  <c:v>88.85</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>88.35</c:v>
+                  <c:v>87.85</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>87.35</c:v>
+                  <c:v>86.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="92373978"/>
-        <c:axId val="2391774"/>
+        <c:axId val="1740101"/>
+        <c:axId val="34135071"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92373978"/>
+        <c:axId val="1740101"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2484,12 +2484,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2391774"/>
+        <c:crossAx val="34135071"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2391774"/>
+        <c:axId val="34135071"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -2535,7 +2535,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92373978"/>
+        <c:crossAx val="1740101"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2583,9 +2583,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>6480</xdr:colOff>
+      <xdr:colOff>6120</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>124920</xdr:rowOff>
+      <xdr:rowOff>124560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2593,8 +2593,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2962080" y="904680"/>
-        <a:ext cx="4340520" cy="2740680"/>
+        <a:off x="2923920" y="904680"/>
+        <a:ext cx="4263840" cy="2740320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2606,16 +2606,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>46080</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>249840</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>184680</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2623,8 +2623,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2693880" y="440640"/>
-        <a:ext cx="8919000" cy="7062120"/>
+        <a:off x="5448240" y="628200"/>
+        <a:ext cx="8776080" cy="7061760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2645,13 +2645,13 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
+      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3163,12 +3163,15 @@
         <v>55.5</v>
       </c>
       <c r="B40" s="0" t="n">
-        <f aca="false">B$2</f>
-        <v>97.45</v>
+        <f aca="false">B39-0.2</f>
+        <v>97.25</v>
       </c>
       <c r="C40" s="0" t="n">
-        <f aca="false">C39</f>
-        <v>97.45</v>
+        <f aca="false">C39-0.2</f>
+        <v>97.25</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3176,12 +3179,12 @@
         <v>57</v>
       </c>
       <c r="B41" s="0" t="n">
-        <f aca="false">B$2</f>
-        <v>97.45</v>
+        <f aca="false">B40-0.2</f>
+        <v>97.05</v>
       </c>
       <c r="C41" s="0" t="n">
-        <f aca="false">C40</f>
-        <v>97.45</v>
+        <f aca="false">C40-0.2</f>
+        <v>97.05</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3189,12 +3192,12 @@
         <v>58.5</v>
       </c>
       <c r="B42" s="0" t="n">
-        <f aca="false">B$2</f>
-        <v>97.45</v>
+        <f aca="false">B41-0.2</f>
+        <v>96.85</v>
       </c>
       <c r="C42" s="0" t="n">
-        <f aca="false">C41</f>
-        <v>97.45</v>
+        <f aca="false">C41-0.2</f>
+        <v>96.85</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3202,12 +3205,12 @@
         <v>60</v>
       </c>
       <c r="B43" s="0" t="n">
-        <f aca="false">B$2</f>
-        <v>97.45</v>
+        <f aca="false">B42-0.2</f>
+        <v>96.65</v>
       </c>
       <c r="C43" s="0" t="n">
-        <f aca="false">C42</f>
-        <v>97.45</v>
+        <f aca="false">C42-0.2</f>
+        <v>96.65</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3215,15 +3218,12 @@
         <v>61.5</v>
       </c>
       <c r="B44" s="0" t="n">
-        <f aca="false">B43-0.1</f>
-        <v>97.35</v>
+        <f aca="false">B43-0.2</f>
+        <v>96.45</v>
       </c>
       <c r="C44" s="0" t="n">
-        <f aca="false">C43-0.1</f>
-        <v>97.35</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>3</v>
+        <f aca="false">C43-0.2</f>
+        <v>96.45</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3231,12 +3231,12 @@
         <v>63</v>
       </c>
       <c r="B45" s="0" t="n">
-        <f aca="false">B44-0.25</f>
-        <v>97.1</v>
+        <f aca="false">B44-0.2</f>
+        <v>96.25</v>
       </c>
       <c r="C45" s="0" t="n">
-        <f aca="false">C44-0.25</f>
-        <v>97.1</v>
+        <f aca="false">C44-0.2</f>
+        <v>96.25</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3244,12 +3244,12 @@
         <v>64.5</v>
       </c>
       <c r="B46" s="0" t="n">
-        <f aca="false">B45-0.25</f>
-        <v>96.85</v>
+        <f aca="false">B45-0.2</f>
+        <v>96.05</v>
       </c>
       <c r="C46" s="0" t="n">
-        <f aca="false">C45-0.25</f>
-        <v>96.85</v>
+        <f aca="false">C45-0.2</f>
+        <v>96.05</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3257,12 +3257,12 @@
         <v>66</v>
       </c>
       <c r="B47" s="0" t="n">
-        <f aca="false">B46-0.25</f>
-        <v>96.6</v>
+        <f aca="false">B46-0.2</f>
+        <v>95.85</v>
       </c>
       <c r="C47" s="0" t="n">
-        <f aca="false">C46-0.25</f>
-        <v>96.6</v>
+        <f aca="false">C46-0.2</f>
+        <v>95.85</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3270,12 +3270,12 @@
         <v>67.5</v>
       </c>
       <c r="B48" s="0" t="n">
-        <f aca="false">B47-0.25</f>
-        <v>96.35</v>
+        <f aca="false">B47-0.2</f>
+        <v>95.65</v>
       </c>
       <c r="C48" s="0" t="n">
-        <f aca="false">C47-0.25</f>
-        <v>96.35</v>
+        <f aca="false">C47-0.2</f>
+        <v>95.65</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3283,12 +3283,12 @@
         <v>69</v>
       </c>
       <c r="B49" s="0" t="n">
-        <f aca="false">B48-0.25</f>
-        <v>96.1</v>
+        <f aca="false">B48-0.2</f>
+        <v>95.45</v>
       </c>
       <c r="C49" s="0" t="n">
-        <f aca="false">C48-0.25</f>
-        <v>96.1</v>
+        <f aca="false">C48-0.2</f>
+        <v>95.45</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3296,12 +3296,12 @@
         <v>70</v>
       </c>
       <c r="B50" s="0" t="n">
-        <f aca="false">B49-0.25</f>
-        <v>95.85</v>
+        <f aca="false">B49-0.2</f>
+        <v>95.25</v>
       </c>
       <c r="C50" s="0" t="n">
-        <f aca="false">C49-0.25</f>
-        <v>95.85</v>
+        <f aca="false">C49-0.2</f>
+        <v>95.25</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3309,12 +3309,12 @@
         <v>71</v>
       </c>
       <c r="B51" s="0" t="n">
-        <f aca="false">B50-0.25</f>
-        <v>95.6</v>
+        <f aca="false">B50-0.2</f>
+        <v>95.05</v>
       </c>
       <c r="C51" s="0" t="n">
-        <f aca="false">C50-0.25</f>
-        <v>95.6</v>
+        <f aca="false">C50-0.2</f>
+        <v>95.05</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3322,12 +3322,12 @@
         <v>72</v>
       </c>
       <c r="B52" s="0" t="n">
-        <f aca="false">B51-0.25</f>
-        <v>95.35</v>
+        <f aca="false">B51-0.2</f>
+        <v>94.85</v>
       </c>
       <c r="C52" s="0" t="n">
-        <f aca="false">C51-0.25</f>
-        <v>95.35</v>
+        <f aca="false">C51-0.2</f>
+        <v>94.85</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3336,11 +3336,11 @@
       </c>
       <c r="B53" s="0" t="n">
         <f aca="false">B52-1</f>
-        <v>94.35</v>
+        <v>93.85</v>
       </c>
       <c r="C53" s="0" t="n">
         <f aca="false">C52-1</f>
-        <v>94.35</v>
+        <v>93.85</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>3</v>
@@ -3352,11 +3352,11 @@
       </c>
       <c r="B54" s="0" t="n">
         <f aca="false">B53-1</f>
-        <v>93.35</v>
+        <v>92.85</v>
       </c>
       <c r="C54" s="0" t="n">
         <f aca="false">C53-1</f>
-        <v>93.35</v>
+        <v>92.85</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3365,11 +3365,11 @@
       </c>
       <c r="B55" s="0" t="n">
         <f aca="false">B54-1</f>
-        <v>92.35</v>
+        <v>91.85</v>
       </c>
       <c r="C55" s="0" t="n">
         <f aca="false">C54-1</f>
-        <v>92.35</v>
+        <v>91.85</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3378,11 +3378,11 @@
       </c>
       <c r="B56" s="0" t="n">
         <f aca="false">B55-1</f>
-        <v>91.35</v>
+        <v>90.85</v>
       </c>
       <c r="C56" s="0" t="n">
         <f aca="false">C55-1</f>
-        <v>91.35</v>
+        <v>90.85</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3391,11 +3391,11 @@
       </c>
       <c r="B57" s="0" t="n">
         <f aca="false">B56-1</f>
-        <v>90.35</v>
+        <v>89.85</v>
       </c>
       <c r="C57" s="0" t="n">
         <f aca="false">C56-1</f>
-        <v>90.35</v>
+        <v>89.85</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3404,11 +3404,11 @@
       </c>
       <c r="B58" s="0" t="n">
         <f aca="false">B57-1</f>
-        <v>89.35</v>
+        <v>88.85</v>
       </c>
       <c r="C58" s="0" t="n">
         <f aca="false">C57-1</f>
-        <v>89.35</v>
+        <v>88.85</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3417,11 +3417,11 @@
       </c>
       <c r="B59" s="0" t="n">
         <f aca="false">B58-1</f>
-        <v>88.35</v>
+        <v>87.85</v>
       </c>
       <c r="C59" s="0" t="n">
         <f aca="false">C58-1</f>
-        <v>88.35</v>
+        <v>87.85</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3430,11 +3430,11 @@
       </c>
       <c r="B60" s="0" t="n">
         <f aca="false">B59-1</f>
-        <v>87.35</v>
+        <v>86.85</v>
       </c>
       <c r="C60" s="0" t="n">
         <f aca="false">C59-1</f>
-        <v>87.35</v>
+        <v>86.85</v>
       </c>
     </row>
   </sheetData>
@@ -3462,7 +3462,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>